<commit_message>
8/6/2025 12:22 AM Commit
</commit_message>
<xml_diff>
--- a/excel/AI Agents fo Data Engineering.xlsx
+++ b/excel/AI Agents fo Data Engineering.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0cbccc594207fa0/Desktop/digeon/digeon/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{A89F7774-AE65-4BF2-9745-D2A10A150E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5934770F-8CDD-4536-A668-C9A67F72F35D}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{A89F7774-AE65-4BF2-9745-D2A10A150E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C3E2DBE-8F66-4899-918E-10CE91BCBF86}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="3640" yWindow="3110" windowWidth="14400" windowHeight="8170" xr2:uid="{237D73BA-908D-44A6-A7C8-918CA8B6AC8F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>AI Agents in Data Engineering</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Open-source / Paid</t>
   </si>
   <si>
-    <t>dbt</t>
-  </si>
-  <si>
     <t>StreamSets</t>
   </si>
   <si>
@@ -162,18 +159,12 @@
     <t>Open-source ETL tool</t>
   </si>
   <si>
-    <t>Pentaho</t>
-  </si>
-  <si>
     <t>Trifacta Wrangler</t>
   </si>
   <si>
     <t>Data wrangling and preparation</t>
   </si>
   <si>
-    <t>Trifacta</t>
-  </si>
-  <si>
     <t>Apache Airflow</t>
   </si>
   <si>
@@ -184,6 +175,66 @@
   </si>
   <si>
     <t>Data quality and validation framework</t>
+  </si>
+  <si>
+    <t>https://datakitchen.io/</t>
+  </si>
+  <si>
+    <t>https://airbyte.com/</t>
+  </si>
+  <si>
+    <t>https://www.fivetran.com/</t>
+  </si>
+  <si>
+    <t>https://dagster.io/</t>
+  </si>
+  <si>
+    <t>https://www.prefect.io/</t>
+  </si>
+  <si>
+    <t>https://www.matillion.com/</t>
+  </si>
+  <si>
+    <t>https://www.talend.com/</t>
+  </si>
+  <si>
+    <t>https://www.getdbt.com/</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/products/streamsets</t>
+  </si>
+  <si>
+    <t>https://nifi.apache.org/</t>
+  </si>
+  <si>
+    <t>https://hevodata.com/</t>
+  </si>
+  <si>
+    <t>https://www.snaplogic.com/</t>
+  </si>
+  <si>
+    <t>https://www.informatica.com/</t>
+  </si>
+  <si>
+    <t>https://admin.google.com/ServiceNotAllowed?application=995920231026&amp;source=scrip&amp;continue=https://cloud.google.com/dataflow</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/glue/</t>
+  </si>
+  <si>
+    <t>https://azure.microsoft.com/en-us/products/data-factory/</t>
+  </si>
+  <si>
+    <t>https://sourceforge.net/projects/pentaho/</t>
+  </si>
+  <si>
+    <t>https://www.alteryx.com/about-us/trifacta-is-now-alteryx-designer-cloud</t>
+  </si>
+  <si>
+    <t>https://airflow.apache.org/</t>
+  </si>
+  <si>
+    <t>https://greatexpectations.io/</t>
   </si>
 </sst>
 </file>
@@ -266,6 +317,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -567,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58279EA9-F5E0-47E5-BCD1-21943C329896}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -609,7 +664,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -623,7 +678,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -637,7 +692,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -651,7 +706,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -665,7 +720,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -679,7 +734,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -693,7 +748,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -707,199 +762,199 @@
         <v>24</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="https://www.datakitchen.io/" xr:uid="{9963E2BB-93F0-47D3-8F9D-BAE961E46892}"/>
-    <hyperlink ref="D4" r:id="rId2" display="https://airbyte.com/" xr:uid="{BA0F1A54-6667-495B-881F-77624DFC8247}"/>
-    <hyperlink ref="D5" r:id="rId3" display="https://fivetran.com/" xr:uid="{5FC1F14A-29EF-4099-92E4-3B979C289DDF}"/>
-    <hyperlink ref="D6" r:id="rId4" display="https://dagster.io/" xr:uid="{42F948AE-336D-470A-B247-E6259C3DB8BE}"/>
-    <hyperlink ref="D7" r:id="rId5" display="https://www.prefect.io/" xr:uid="{08DEEB61-98AE-4825-AF44-183DEBBCDF83}"/>
-    <hyperlink ref="D8" r:id="rId6" display="https://www.matillion.com/" xr:uid="{F32F5A2F-B06D-4971-9679-D226982D80B4}"/>
-    <hyperlink ref="D9" r:id="rId7" display="https://www.talend.com/" xr:uid="{74F70B73-0109-4195-84F9-6E09B8CFCB89}"/>
-    <hyperlink ref="D10" r:id="rId8" display="https://www.getdbt.com/" xr:uid="{866F876C-43C0-4FFC-81C5-9A5913E20FE4}"/>
-    <hyperlink ref="D11" r:id="rId9" display="https://streamsets.com/" xr:uid="{E256C13E-85C7-43D0-BB07-97268FF94F70}"/>
-    <hyperlink ref="D12" r:id="rId10" display="https://nifi.apache.org/" xr:uid="{55AC05EF-50FD-47A0-91C5-80926A30CB02}"/>
-    <hyperlink ref="D13" r:id="rId11" display="https://hevodata.com/" xr:uid="{37DB7317-443C-43EC-A4B7-3CEEA8720858}"/>
-    <hyperlink ref="D14" r:id="rId12" display="https://www.snaplogic.com/" xr:uid="{3E7D45F7-9E6D-4A7C-B499-DCDFD71793BA}"/>
-    <hyperlink ref="D15" r:id="rId13" display="https://www.informatica.com/" xr:uid="{F648AB42-50E5-480A-97DC-BE744A49D819}"/>
-    <hyperlink ref="D16" r:id="rId14" display="https://cloud.google.com/dataflow" xr:uid="{D7504A31-FE4F-4477-962A-6173384AEE75}"/>
-    <hyperlink ref="D17" r:id="rId15" display="https://aws.amazon.com/glue/" xr:uid="{B8868D88-908D-416E-B707-E7065CCF5CC8}"/>
-    <hyperlink ref="D18" r:id="rId16" display="https://azure.microsoft.com/en-us/services/data-factory/" xr:uid="{29335292-140F-4E95-B128-096C7BFD6D47}"/>
-    <hyperlink ref="D19" r:id="rId17" display="https://sourceforge.net/projects/pentaho/" xr:uid="{863489B8-9C49-4857-B123-B0D8C6284F56}"/>
-    <hyperlink ref="D20" r:id="rId18" display="https://www.trifacta.com/" xr:uid="{39F11656-1521-4B8C-A188-B4E5AB67C647}"/>
-    <hyperlink ref="D21" r:id="rId19" display="https://airflow.apache.org/" xr:uid="{3E0132E2-431A-403C-8C8D-60C2FE7B9FBB}"/>
-    <hyperlink ref="D22" r:id="rId20" display="https://greatexpectations.io/" xr:uid="{5DC3F18C-598C-48C9-98B4-DAC38AD28B0F}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{9963E2BB-93F0-47D3-8F9D-BAE961E46892}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{BA0F1A54-6667-495B-881F-77624DFC8247}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{5FC1F14A-29EF-4099-92E4-3B979C289DDF}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{42F948AE-336D-470A-B247-E6259C3DB8BE}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{08DEEB61-98AE-4825-AF44-183DEBBCDF83}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{F32F5A2F-B06D-4971-9679-D226982D80B4}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{74F70B73-0109-4195-84F9-6E09B8CFCB89}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{866F876C-43C0-4FFC-81C5-9A5913E20FE4}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{E256C13E-85C7-43D0-BB07-97268FF94F70}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{55AC05EF-50FD-47A0-91C5-80926A30CB02}"/>
+    <hyperlink ref="D13" r:id="rId11" xr:uid="{37DB7317-443C-43EC-A4B7-3CEEA8720858}"/>
+    <hyperlink ref="D14" r:id="rId12" xr:uid="{3E7D45F7-9E6D-4A7C-B499-DCDFD71793BA}"/>
+    <hyperlink ref="D15" r:id="rId13" xr:uid="{F648AB42-50E5-480A-97DC-BE744A49D819}"/>
+    <hyperlink ref="D16" r:id="rId14" xr:uid="{D7504A31-FE4F-4477-962A-6173384AEE75}"/>
+    <hyperlink ref="D17" r:id="rId15" xr:uid="{B8868D88-908D-416E-B707-E7065CCF5CC8}"/>
+    <hyperlink ref="D18" r:id="rId16" xr:uid="{29335292-140F-4E95-B128-096C7BFD6D47}"/>
+    <hyperlink ref="D19" r:id="rId17" xr:uid="{863489B8-9C49-4857-B123-B0D8C6284F56}"/>
+    <hyperlink ref="D20" r:id="rId18" xr:uid="{39F11656-1521-4B8C-A188-B4E5AB67C647}"/>
+    <hyperlink ref="D21" r:id="rId19" xr:uid="{3E0132E2-431A-403C-8C8D-60C2FE7B9FBB}"/>
+    <hyperlink ref="D22" r:id="rId20" xr:uid="{5DC3F18C-598C-48C9-98B4-DAC38AD28B0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>